<commit_message>
Ajuste da formatação dos ips na planilha gravadores
</commit_message>
<xml_diff>
--- a/gravadores.xlsx
+++ b/gravadores.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Python\monitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09F04A8-CCA6-4DA0-BF1E-2565773F908E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8361C46A-870A-4908-B395-C6EA608C3594}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8964" xr2:uid="{ECEBB141-BA45-4E9E-A807-4CD3B5308026}"/>
   </bookViews>
   <sheets>
     <sheet name="gravadores" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">gravadores!$A$1:$F$94</definedName>
+  </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="314">
   <si>
     <t>nome</t>
   </si>
@@ -807,9 +810,6 @@
     <t>187.76.11.72</t>
   </si>
   <si>
-    <t>DIVINOPOLIS</t>
-  </si>
-  <si>
     <t>MG-MCL-CEN</t>
   </si>
   <si>
@@ -892,6 +892,84 @@
   </si>
   <si>
     <t>ip</t>
+  </si>
+  <si>
+    <t>200.202.197.102</t>
+  </si>
+  <si>
+    <t>SÃO JOÃO DE MERITI</t>
+  </si>
+  <si>
+    <t>200.223.200.118</t>
+  </si>
+  <si>
+    <t>37777</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>200.202.243.240</t>
+  </si>
+  <si>
+    <t>200.149.101.176</t>
+  </si>
+  <si>
+    <t>RIBEIRÃO DAS NEVES</t>
+  </si>
+  <si>
+    <t>200.164.236.106</t>
+  </si>
+  <si>
+    <t>50000</t>
+  </si>
+  <si>
+    <t>200.222.142.250</t>
+  </si>
+  <si>
+    <t>200.165.139.102</t>
+  </si>
+  <si>
+    <t>200.222.100.154</t>
+  </si>
+  <si>
+    <t>200.216.246.102</t>
+  </si>
+  <si>
+    <t>200.216.241.234</t>
+  </si>
+  <si>
+    <t>200.149.223.114</t>
+  </si>
+  <si>
+    <t>200.149.213.130</t>
+  </si>
+  <si>
+    <t>169.254.245.206</t>
+  </si>
+  <si>
+    <t>179.255.254.206</t>
+  </si>
+  <si>
+    <t>200.216.240.240</t>
+  </si>
+  <si>
+    <t>200.216.163.186</t>
+  </si>
+  <si>
+    <t>200.202.243.233</t>
+  </si>
+  <si>
+    <t>200.223.164.248</t>
+  </si>
+  <si>
+    <t>200.222.107.250</t>
+  </si>
+  <si>
+    <t>200.164.148.122</t>
+  </si>
+  <si>
+    <t>200.141.233.144</t>
   </si>
 </sst>
 </file>
@@ -927,7 +1005,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -935,14 +1013,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1252,16 +1362,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04D08327-CC56-40E1-9DD9-645D25F2751F}">
-  <dimension ref="A1:F119"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
+      <selection activeCell="A116" sqref="A116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.6640625" bestFit="1" customWidth="1"/>
@@ -1273,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -1310,16 +1420,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3">
-        <v>200202197102</v>
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
       </c>
       <c r="C3">
         <v>50000</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -1330,16 +1440,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C4">
         <v>50000</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -1350,19 +1460,19 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C5">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -1370,19 +1480,19 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C6">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D6" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -1390,19 +1500,19 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C7">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -1410,19 +1520,19 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C8">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F8">
         <v>1</v>
@@ -1430,19 +1540,19 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C9">
         <v>50000</v>
       </c>
       <c r="D9" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -1450,16 +1560,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C10">
         <v>50000</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -1470,16 +1580,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C11">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -1490,19 +1600,19 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C12">
         <v>37777</v>
       </c>
       <c r="D12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1510,16 +1620,16 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>37777</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
         <v>8</v>
@@ -1530,19 +1640,19 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C14">
         <v>37777</v>
       </c>
       <c r="D14" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -1550,19 +1660,19 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C15">
         <v>37777</v>
       </c>
       <c r="D15" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -1570,19 +1680,19 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C16">
         <v>37777</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>10</v>
       </c>
       <c r="E16" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -1590,19 +1700,19 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C17">
         <v>37777</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -1610,19 +1720,19 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C18">
         <v>37777</v>
       </c>
       <c r="D18" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F18">
         <v>1</v>
@@ -1630,16 +1740,16 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C19">
         <v>37777</v>
       </c>
       <c r="D19" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
@@ -1650,16 +1760,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C20">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
@@ -1670,13 +1780,13 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C21">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D21" t="s">
         <v>14</v>
@@ -1690,19 +1800,19 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>62</v>
-      </c>
-      <c r="B22" s="3">
-        <v>200223200118</v>
+        <v>65</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>66</v>
       </c>
       <c r="C22">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D22" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="E22" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F22">
         <v>1</v>
@@ -1710,10 +1820,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="C23">
         <v>37777</v>
@@ -1730,16 +1840,16 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C24">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D24" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="E24" t="s">
         <v>8</v>
@@ -1750,19 +1860,19 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C25">
         <v>37777</v>
       </c>
       <c r="D25" t="s">
-        <v>14</v>
+        <v>74</v>
       </c>
       <c r="E25" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -1770,19 +1880,19 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="C26">
         <v>37777</v>
       </c>
       <c r="D26" t="s">
-        <v>7</v>
+        <v>77</v>
       </c>
       <c r="E26" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -1790,19 +1900,19 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="C27">
         <v>37777</v>
       </c>
       <c r="D27" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="E27" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1810,19 +1920,19 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="C28">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="E28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F28">
         <v>1</v>
@@ -1830,19 +1940,19 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>61</v>
+        <v>84</v>
       </c>
       <c r="C29">
         <v>37777</v>
       </c>
       <c r="D29" t="s">
-        <v>79</v>
+        <v>85</v>
       </c>
       <c r="E29" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F29">
         <v>1</v>
@@ -1850,16 +1960,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="C30">
         <v>50000</v>
       </c>
       <c r="D30" t="s">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="E30" t="s">
         <v>8</v>
@@ -1870,16 +1980,16 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="C31">
         <v>37777</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
@@ -1890,16 +2000,16 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C32">
         <v>50000</v>
       </c>
       <c r="D32" t="s">
-        <v>40</v>
+        <v>93</v>
       </c>
       <c r="E32" t="s">
         <v>8</v>
@@ -1910,16 +2020,16 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>88</v>
-      </c>
-      <c r="B33" s="3">
-        <v>200202243240</v>
+        <v>94</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="C33">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D33" t="s">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
@@ -1930,16 +2040,16 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C34">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D34" t="s">
-        <v>7</v>
+        <v>99</v>
       </c>
       <c r="E34" t="s">
         <v>8</v>
@@ -1950,16 +2060,16 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="C35">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D35" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="E35" t="s">
         <v>8</v>
@@ -1970,19 +2080,19 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="C36">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -1990,19 +2100,19 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="C37">
         <v>50000</v>
       </c>
       <c r="D37" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="E37" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="F37">
         <v>1</v>
@@ -2010,19 +2120,19 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>100</v>
-      </c>
-      <c r="B38" s="3">
-        <v>200149101176</v>
+        <v>111</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="C38">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D38" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
       <c r="E38" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="F38">
         <v>1</v>
@@ -2030,19 +2140,19 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="C39">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D39" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="E39" t="s">
-        <v>8</v>
+        <v>116</v>
       </c>
       <c r="F39">
         <v>1</v>
@@ -2050,16 +2160,16 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="C40">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="E40" t="s">
         <v>11</v>
@@ -2070,19 +2180,19 @@
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="C41">
         <v>50000</v>
       </c>
       <c r="D41" t="s">
-        <v>109</v>
+        <v>14</v>
       </c>
       <c r="E41" t="s">
-        <v>110</v>
+        <v>11</v>
       </c>
       <c r="F41">
         <v>1</v>
@@ -2090,19 +2200,19 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="C42">
         <v>50000</v>
       </c>
       <c r="D42" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="E42" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -2110,19 +2220,19 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>135</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="C43">
         <v>50000</v>
       </c>
       <c r="D43" t="s">
-        <v>115</v>
+        <v>7</v>
       </c>
       <c r="E43" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -2130,19 +2240,19 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>117</v>
+        <v>137</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="C44">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D44" t="s">
-        <v>119</v>
+        <v>7</v>
       </c>
       <c r="E44" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F44">
         <v>1</v>
@@ -2150,19 +2260,19 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="3">
-        <v>200164236106</v>
+        <v>139</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>140</v>
       </c>
       <c r="C45">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D45" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="E45" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F45">
         <v>1</v>
@@ -2170,19 +2280,19 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>122</v>
-      </c>
-      <c r="B46" s="3">
-        <v>200222142250</v>
+        <v>143</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="C46">
         <v>50000</v>
       </c>
       <c r="D46" t="s">
-        <v>123</v>
+        <v>145</v>
       </c>
       <c r="E46" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -2190,19 +2300,19 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>124</v>
-      </c>
-      <c r="B47" s="3">
-        <v>200165139102</v>
+        <v>148</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>149</v>
       </c>
       <c r="C47">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D47" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="E47" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -2210,19 +2320,19 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="C48">
         <v>50000</v>
       </c>
       <c r="D48" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="E48" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F48">
         <v>1</v>
@@ -2230,19 +2340,19 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>128</v>
+        <v>153</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
       <c r="C49">
         <v>50000</v>
       </c>
       <c r="D49" t="s">
-        <v>130</v>
+        <v>155</v>
       </c>
       <c r="E49" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F49">
         <v>1</v>
@@ -2250,19 +2360,19 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>131</v>
-      </c>
-      <c r="B50" s="3">
-        <v>200222100154</v>
+        <v>156</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>157</v>
       </c>
       <c r="C50">
         <v>50000</v>
       </c>
       <c r="D50" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="E50" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F50">
         <v>1</v>
@@ -2270,19 +2380,19 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>133</v>
-      </c>
-      <c r="B51" s="3">
-        <v>200216246102</v>
+        <v>159</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="C51">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D51" t="s">
-        <v>134</v>
+        <v>161</v>
       </c>
       <c r="E51" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -2290,19 +2400,19 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="C52">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D52" t="s">
-        <v>7</v>
+        <v>164</v>
       </c>
       <c r="E52" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F52">
         <v>1</v>
@@ -2310,19 +2420,19 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>137</v>
+        <v>169</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="C53">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D53" t="s">
-        <v>7</v>
+        <v>109</v>
       </c>
       <c r="E53" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -2330,19 +2440,19 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>140</v>
+        <v>173</v>
       </c>
       <c r="C54">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D54" t="s">
-        <v>7</v>
+        <v>174</v>
       </c>
       <c r="E54" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F54">
         <v>1</v>
@@ -2350,19 +2460,19 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>141</v>
-      </c>
-      <c r="B55" s="3">
-        <v>200216241234</v>
+        <v>175</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>176</v>
       </c>
       <c r="C55">
         <v>50000</v>
       </c>
       <c r="D55" t="s">
-        <v>142</v>
+        <v>109</v>
       </c>
       <c r="E55" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -2370,19 +2480,19 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>143</v>
+        <v>177</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>144</v>
+        <v>178</v>
       </c>
       <c r="C56">
         <v>50000</v>
       </c>
       <c r="D56" t="s">
-        <v>145</v>
+        <v>22</v>
       </c>
       <c r="E56" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -2390,19 +2500,19 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>146</v>
-      </c>
-      <c r="B57" s="3">
-        <v>200149223114</v>
+        <v>179</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>180</v>
       </c>
       <c r="C57">
         <v>50000</v>
       </c>
       <c r="D57" t="s">
-        <v>147</v>
+        <v>22</v>
       </c>
       <c r="E57" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F57">
         <v>1</v>
@@ -2410,19 +2520,19 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>148</v>
+        <v>181</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>149</v>
+        <v>182</v>
       </c>
       <c r="C58">
         <v>50000</v>
       </c>
       <c r="D58" t="s">
-        <v>7</v>
+        <v>183</v>
       </c>
       <c r="E58" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -2430,13 +2540,13 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="C59">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D59" t="s">
         <v>7</v>
@@ -2450,19 +2560,19 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>152</v>
-      </c>
-      <c r="B60" s="3">
-        <v>200149213130</v>
+        <v>186</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>187</v>
       </c>
       <c r="C60">
         <v>50000</v>
       </c>
       <c r="D60" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="E60" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F60">
         <v>1</v>
@@ -2470,19 +2580,19 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>153</v>
+        <v>188</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="C61">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D61" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="E61" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -2490,16 +2600,16 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="C62">
         <v>50000</v>
       </c>
       <c r="D62" t="s">
-        <v>158</v>
+        <v>193</v>
       </c>
       <c r="E62" t="s">
         <v>11</v>
@@ -2510,19 +2620,19 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>159</v>
+        <v>194</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>160</v>
+        <v>195</v>
       </c>
       <c r="C63">
         <v>37777</v>
       </c>
       <c r="D63" t="s">
-        <v>161</v>
+        <v>196</v>
       </c>
       <c r="E63" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -2530,19 +2640,19 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>162</v>
+        <v>197</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>163</v>
+        <v>198</v>
       </c>
       <c r="C64">
         <v>37777</v>
       </c>
       <c r="D64" t="s">
-        <v>164</v>
+        <v>7</v>
       </c>
       <c r="E64" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F64">
         <v>1</v>
@@ -2550,19 +2660,19 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>165</v>
-      </c>
-      <c r="B65" s="3">
-        <v>169254245206</v>
+        <v>199</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="C65">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D65" t="s">
-        <v>166</v>
+        <v>130</v>
       </c>
       <c r="E65" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="F65">
         <v>1</v>
@@ -2570,19 +2680,19 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>167</v>
-      </c>
-      <c r="B66" s="3">
-        <v>169254245206</v>
+        <v>201</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="C66">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D66" t="s">
-        <v>168</v>
+        <v>203</v>
       </c>
       <c r="E66" t="s">
-        <v>116</v>
+        <v>8</v>
       </c>
       <c r="F66">
         <v>1</v>
@@ -2590,19 +2700,19 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>169</v>
+        <v>204</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="C67">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D67" t="s">
-        <v>109</v>
+        <v>40</v>
       </c>
       <c r="E67" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -2610,19 +2720,19 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>171</v>
-      </c>
-      <c r="B68" s="3">
-        <v>179255254206</v>
+        <v>206</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="C68">
         <v>37777</v>
       </c>
       <c r="D68" t="s">
-        <v>109</v>
+        <v>7</v>
       </c>
       <c r="E68" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -2630,19 +2740,19 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="C69">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D69" t="s">
-        <v>174</v>
+        <v>67</v>
       </c>
       <c r="E69" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -2650,19 +2760,19 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>175</v>
+        <v>214</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>176</v>
+        <v>215</v>
       </c>
       <c r="C70">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D70" t="s">
-        <v>109</v>
+        <v>216</v>
       </c>
       <c r="E70" t="s">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -2670,19 +2780,19 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>177</v>
+        <v>217</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>178</v>
+        <v>218</v>
       </c>
       <c r="C71">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D71" t="s">
-        <v>22</v>
+        <v>96</v>
       </c>
       <c r="E71" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -2690,19 +2800,19 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>179</v>
+        <v>221</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>180</v>
+        <v>222</v>
       </c>
       <c r="C72">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D72" t="s">
-        <v>22</v>
+        <v>223</v>
       </c>
       <c r="E72" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="F72">
         <v>1</v>
@@ -2710,19 +2820,19 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>181</v>
+        <v>224</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>182</v>
+        <v>225</v>
       </c>
       <c r="C73">
         <v>50000</v>
       </c>
       <c r="D73" t="s">
-        <v>183</v>
+        <v>226</v>
       </c>
       <c r="E73" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -2730,19 +2840,19 @@
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>184</v>
+        <v>229</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>185</v>
+        <v>230</v>
       </c>
       <c r="C74">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D74" t="s">
-        <v>7</v>
+        <v>228</v>
       </c>
       <c r="E74" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -2750,19 +2860,19 @@
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>186</v>
+        <v>231</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>187</v>
+        <v>232</v>
       </c>
       <c r="C75">
         <v>50000</v>
       </c>
       <c r="D75" t="s">
-        <v>7</v>
+        <v>233</v>
       </c>
       <c r="E75" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -2770,19 +2880,19 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>188</v>
+        <v>234</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>189</v>
+        <v>235</v>
       </c>
       <c r="C76">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D76" t="s">
-        <v>190</v>
+        <v>14</v>
       </c>
       <c r="E76" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -2790,19 +2900,19 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>191</v>
+        <v>237</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>192</v>
+        <v>238</v>
       </c>
       <c r="C77">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D77" t="s">
-        <v>193</v>
+        <v>101</v>
       </c>
       <c r="E77" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -2810,16 +2920,16 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>194</v>
+        <v>239</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>195</v>
+        <v>240</v>
       </c>
       <c r="C78">
         <v>37777</v>
       </c>
       <c r="D78" t="s">
-        <v>196</v>
+        <v>241</v>
       </c>
       <c r="E78" t="s">
         <v>8</v>
@@ -2830,13 +2940,13 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>197</v>
+        <v>242</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>198</v>
+        <v>243</v>
       </c>
       <c r="C79">
-        <v>37777</v>
+        <v>50000</v>
       </c>
       <c r="D79" t="s">
         <v>7</v>
@@ -2850,16 +2960,16 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>199</v>
+        <v>244</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>200</v>
+        <v>245</v>
       </c>
       <c r="C80">
         <v>37777</v>
       </c>
       <c r="D80" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="E80" t="s">
         <v>8</v>
@@ -2870,16 +2980,16 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>201</v>
+        <v>246</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>202</v>
+        <v>247</v>
       </c>
       <c r="C81">
         <v>37777</v>
       </c>
       <c r="D81" t="s">
-        <v>203</v>
+        <v>7</v>
       </c>
       <c r="E81" t="s">
         <v>8</v>
@@ -2890,16 +3000,16 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>204</v>
+        <v>248</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>205</v>
+        <v>249</v>
       </c>
       <c r="C82">
         <v>37777</v>
       </c>
       <c r="D82" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E82" t="s">
         <v>8</v>
@@ -2910,16 +3020,16 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>206</v>
+        <v>250</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>207</v>
+        <v>251</v>
       </c>
       <c r="C83">
         <v>37777</v>
       </c>
       <c r="D83" t="s">
-        <v>7</v>
+        <v>252</v>
       </c>
       <c r="E83" t="s">
         <v>8</v>
@@ -2930,16 +3040,16 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>208</v>
-      </c>
-      <c r="B84" s="3">
-        <v>200216240240</v>
+        <v>253</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>254</v>
       </c>
       <c r="C84">
         <v>37777</v>
       </c>
       <c r="D84" t="s">
-        <v>7</v>
+        <v>255</v>
       </c>
       <c r="E84" t="s">
         <v>8</v>
@@ -2950,16 +3060,16 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>209</v>
-      </c>
-      <c r="B85" s="3">
-        <v>200216163186</v>
+        <v>256</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>257</v>
       </c>
       <c r="C85">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D85" t="s">
-        <v>7</v>
+        <v>67</v>
       </c>
       <c r="E85" t="s">
         <v>8</v>
@@ -2970,19 +3080,19 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>210</v>
+        <v>268</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>211</v>
+        <v>269</v>
       </c>
       <c r="C86">
         <v>37777</v>
       </c>
       <c r="D86" t="s">
-        <v>67</v>
+        <v>270</v>
       </c>
       <c r="E86" t="s">
-        <v>8</v>
+        <v>267</v>
       </c>
       <c r="F86">
         <v>1</v>
@@ -2990,19 +3100,19 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>212</v>
-      </c>
-      <c r="B87" s="3">
-        <v>200202243233</v>
+        <v>271</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>272</v>
       </c>
       <c r="C87">
         <v>37777</v>
       </c>
       <c r="D87" t="s">
-        <v>213</v>
+        <v>273</v>
       </c>
       <c r="E87" t="s">
-        <v>8</v>
+        <v>267</v>
       </c>
       <c r="F87">
         <v>1</v>
@@ -3010,19 +3120,19 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>214</v>
+        <v>274</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>215</v>
+        <v>275</v>
       </c>
       <c r="C88">
         <v>37777</v>
       </c>
       <c r="D88" t="s">
-        <v>216</v>
+        <v>276</v>
       </c>
       <c r="E88" t="s">
-        <v>8</v>
+        <v>267</v>
       </c>
       <c r="F88">
         <v>1</v>
@@ -3030,19 +3140,19 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>217</v>
+        <v>277</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>218</v>
+        <v>278</v>
       </c>
       <c r="C89">
         <v>37777</v>
       </c>
       <c r="D89" t="s">
-        <v>96</v>
+        <v>279</v>
       </c>
       <c r="E89" t="s">
-        <v>8</v>
+        <v>267</v>
       </c>
       <c r="F89">
         <v>1</v>
@@ -3050,19 +3160,19 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>219</v>
-      </c>
-      <c r="B90" s="3">
-        <v>200223164248</v>
+        <v>280</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>281</v>
       </c>
       <c r="C90">
         <v>37777</v>
       </c>
       <c r="D90" t="s">
-        <v>220</v>
+        <v>282</v>
       </c>
       <c r="E90" t="s">
-        <v>8</v>
+        <v>267</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -3070,19 +3180,19 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>221</v>
+        <v>283</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>222</v>
+        <v>284</v>
       </c>
       <c r="C91">
         <v>37777</v>
       </c>
       <c r="D91" t="s">
-        <v>223</v>
+        <v>285</v>
       </c>
       <c r="E91" t="s">
-        <v>8</v>
+        <v>267</v>
       </c>
       <c r="F91">
         <v>1</v>
@@ -3090,19 +3200,19 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>224</v>
+        <v>263</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>225</v>
+        <v>264</v>
       </c>
       <c r="C92">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D92" t="s">
-        <v>226</v>
+        <v>48</v>
       </c>
       <c r="E92" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -3110,19 +3220,19 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>227</v>
-      </c>
-      <c r="B93" s="3">
-        <v>200222107250</v>
+        <v>260</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>261</v>
       </c>
       <c r="C93">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D93" t="s">
-        <v>228</v>
+        <v>262</v>
       </c>
       <c r="E93" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F93">
         <v>1</v>
@@ -3130,19 +3240,19 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>229</v>
+        <v>258</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>230</v>
+        <v>259</v>
       </c>
       <c r="C94">
-        <v>50000</v>
+        <v>37777</v>
       </c>
       <c r="D94" t="s">
-        <v>228</v>
+        <v>286</v>
       </c>
       <c r="E94" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -3150,16 +3260,16 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>231</v>
-      </c>
-      <c r="B95" s="2" t="s">
-        <v>232</v>
+        <v>9</v>
+      </c>
+      <c r="B95" s="4" t="s">
+        <v>288</v>
       </c>
       <c r="C95">
         <v>50000</v>
       </c>
       <c r="D95" t="s">
-        <v>233</v>
+        <v>289</v>
       </c>
       <c r="E95" t="s">
         <v>11</v>
@@ -3168,487 +3278,449 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>234</v>
-      </c>
-      <c r="B96" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C96">
-        <v>50000</v>
-      </c>
-      <c r="D96" t="s">
+    <row r="96" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="C96" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B97" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C97" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E97" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B98" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="C98" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D98" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="E98" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B99" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="C99" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D99" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E99" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C100" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D100" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E100" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B101" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="C101" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D101" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E101" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B102" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D102" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B103" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D103" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E103" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B104" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B105" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="C105" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D105" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="E105" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B106" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="C106" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D106" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E106" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D107" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D108" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="E108" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A110" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D110" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E110" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E111" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="s">
+        <v>212</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D112" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="E112" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D113" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D114" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="E114" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D115" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E96" t="s">
+      <c r="E115" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F96">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A97" t="s">
-        <v>236</v>
-      </c>
-      <c r="B97" s="3">
-        <v>200164148122</v>
-      </c>
-      <c r="C97">
-        <v>50000</v>
-      </c>
-      <c r="D97" t="s">
-        <v>14</v>
-      </c>
-      <c r="E97" t="s">
-        <v>11</v>
-      </c>
-      <c r="F97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>237</v>
-      </c>
-      <c r="B98" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="C98">
-        <v>37777</v>
-      </c>
-      <c r="D98" t="s">
-        <v>101</v>
-      </c>
-      <c r="E98" t="s">
-        <v>8</v>
-      </c>
-      <c r="F98">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>239</v>
-      </c>
-      <c r="B99" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="C99">
-        <v>37777</v>
-      </c>
-      <c r="D99" t="s">
-        <v>241</v>
-      </c>
-      <c r="E99" t="s">
-        <v>8</v>
-      </c>
-      <c r="F99">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>242</v>
-      </c>
-      <c r="B100" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C100">
-        <v>50000</v>
-      </c>
-      <c r="D100" t="s">
-        <v>7</v>
-      </c>
-      <c r="E100" t="s">
-        <v>8</v>
-      </c>
-      <c r="F100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>244</v>
-      </c>
-      <c r="B101" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="C101">
-        <v>37777</v>
-      </c>
-      <c r="D101" t="s">
-        <v>7</v>
-      </c>
-      <c r="E101" t="s">
-        <v>8</v>
-      </c>
-      <c r="F101">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>246</v>
-      </c>
-      <c r="B102" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="C102">
-        <v>37777</v>
-      </c>
-      <c r="D102" t="s">
-        <v>7</v>
-      </c>
-      <c r="E102" t="s">
-        <v>8</v>
-      </c>
-      <c r="F102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>248</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="C103">
-        <v>37777</v>
-      </c>
-      <c r="D103" t="s">
-        <v>7</v>
-      </c>
-      <c r="E103" t="s">
-        <v>8</v>
-      </c>
-      <c r="F103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>250</v>
-      </c>
-      <c r="B104" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="C104">
-        <v>37777</v>
-      </c>
-      <c r="D104" t="s">
-        <v>252</v>
-      </c>
-      <c r="E104" t="s">
-        <v>8</v>
-      </c>
-      <c r="F104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>253</v>
-      </c>
-      <c r="B105" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="C105">
-        <v>37777</v>
-      </c>
-      <c r="D105" t="s">
-        <v>255</v>
-      </c>
-      <c r="E105" t="s">
-        <v>8</v>
-      </c>
-      <c r="F105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>256</v>
-      </c>
-      <c r="B106" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="C106">
-        <v>37777</v>
-      </c>
-      <c r="D106" t="s">
-        <v>67</v>
-      </c>
-      <c r="E106" t="s">
-        <v>8</v>
-      </c>
-      <c r="F106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>258</v>
-      </c>
-      <c r="B107" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C107">
-        <v>37777</v>
-      </c>
-      <c r="D107" t="s">
-        <v>260</v>
-      </c>
-      <c r="E107" t="s">
-        <v>8</v>
-      </c>
-      <c r="F107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>261</v>
-      </c>
-      <c r="B108" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C108">
-        <v>37777</v>
-      </c>
-      <c r="D108" t="s">
-        <v>263</v>
-      </c>
-      <c r="E108" t="s">
-        <v>8</v>
-      </c>
-      <c r="F108">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>264</v>
-      </c>
-      <c r="B109" s="2" t="s">
+      <c r="F115" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="C109">
-        <v>37777</v>
-      </c>
-      <c r="D109" t="s">
-        <v>48</v>
-      </c>
-      <c r="E109" t="s">
-        <v>8</v>
-      </c>
-      <c r="F109">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+      <c r="B116" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D116" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="B110" s="3">
-        <v>200141233144</v>
-      </c>
-      <c r="C110">
-        <v>37777</v>
-      </c>
-      <c r="D110" t="s">
+      <c r="E116" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="E110" t="s">
-        <v>268</v>
-      </c>
-      <c r="F110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>269</v>
-      </c>
-      <c r="B111" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="C111">
-        <v>37777</v>
-      </c>
-      <c r="D111" t="s">
-        <v>271</v>
-      </c>
-      <c r="E111" t="s">
-        <v>268</v>
-      </c>
-      <c r="F111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
-        <v>272</v>
-      </c>
-      <c r="B112" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="C112">
-        <v>37777</v>
-      </c>
-      <c r="D112" t="s">
-        <v>274</v>
-      </c>
-      <c r="E112" t="s">
-        <v>268</v>
-      </c>
-      <c r="F112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>275</v>
-      </c>
-      <c r="B113" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="C113">
-        <v>37777</v>
-      </c>
-      <c r="D113" t="s">
-        <v>277</v>
-      </c>
-      <c r="E113" t="s">
-        <v>268</v>
-      </c>
-      <c r="F113">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>278</v>
-      </c>
-      <c r="B114" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="C114">
-        <v>37777</v>
-      </c>
-      <c r="D114" t="s">
-        <v>280</v>
-      </c>
-      <c r="E114" t="s">
-        <v>268</v>
-      </c>
-      <c r="F114">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>281</v>
-      </c>
-      <c r="B115" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="C115">
-        <v>37777</v>
-      </c>
-      <c r="D115" t="s">
-        <v>283</v>
-      </c>
-      <c r="E115" t="s">
-        <v>268</v>
-      </c>
-      <c r="F115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A116" t="s">
-        <v>284</v>
-      </c>
-      <c r="B116" s="2" t="s">
-        <v>285</v>
-      </c>
-      <c r="C116">
-        <v>37777</v>
-      </c>
-      <c r="D116" t="s">
-        <v>286</v>
-      </c>
-      <c r="E116" t="s">
-        <v>268</v>
-      </c>
-      <c r="F116">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A117" t="s">
-        <v>264</v>
-      </c>
-      <c r="B117" s="2" t="s">
-        <v>265</v>
-      </c>
-      <c r="C117">
-        <v>37777</v>
-      </c>
-      <c r="D117" t="s">
-        <v>48</v>
-      </c>
-      <c r="E117" t="s">
-        <v>8</v>
-      </c>
-      <c r="F117">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A118" t="s">
-        <v>261</v>
-      </c>
-      <c r="B118" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="C118">
-        <v>37777</v>
-      </c>
-      <c r="D118" t="s">
-        <v>263</v>
-      </c>
-      <c r="E118" t="s">
-        <v>8</v>
-      </c>
-      <c r="F118">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A119" t="s">
-        <v>258</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="C119">
-        <v>37777</v>
-      </c>
-      <c r="D119" t="s">
-        <v>287</v>
-      </c>
-      <c r="E119" t="s">
-        <v>8</v>
-      </c>
-      <c r="F119">
-        <v>1</v>
-      </c>
-    </row>
+      <c r="F116" s="4" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="126" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="129" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" s="4" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
+  <autoFilter ref="A1:F94" xr:uid="{0F48D705-A654-4A80-B4F7-FD74AC89DC55}"/>
+  <conditionalFormatting sqref="B1:B1048576">
+    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>